<commit_message>
add non-resident data for 2019-2021 to reports, script, exported csv. add corresponding plot to published index.html. Update readme files
</commit_message>
<xml_diff>
--- a/External Data/reports/2019_termination_data.xlsx
+++ b/External Data/reports/2019_termination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TedSc\OneDrive\Desktop\R Projects\indiana_abortion\External Data\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19154E-90B3-44B7-A9D3-2769BBF23099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB02B162-58CF-410D-9995-4863B7A62A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="360" windowWidth="14460" windowHeight="9925" tabRatio="821" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" tabRatio="821" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019_age" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="2019_monthly" sheetId="13" r:id="rId11"/>
     <sheet name="2019_procedure_location_wrksht" sheetId="12" r:id="rId12"/>
     <sheet name="2019_gestation_weeks" sheetId="11" r:id="rId13"/>
+    <sheet name="2019_non_res" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="206">
   <si>
     <t>Age, years</t>
   </si>
@@ -645,6 +646,24 @@
   </si>
   <si>
     <t>26 (.34%)</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>abortions</t>
   </si>
 </sst>
 </file>
@@ -2270,7 +2289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDE9370-27EA-44DC-94C9-B28100D1EBB8}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2917,6 +2936,77 @@
       </c>
       <c r="C19" s="9">
         <v>7.8564881497970404E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2A9DA4-CF71-4D41-9CDA-9716BC618EB7}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>